<commit_message>
added paiements and generate excel. payment columns filled, date sorted
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Nom :</t>
   </si>
   <si>
-    <t>LOIC</t>
+    <t>AGNOLETTO VITTORIA</t>
   </si>
   <si>
     <t>Date</t>
@@ -51,6 +51,30 @@
   </si>
   <si>
     <t>Solde</t>
+  </si>
+  <si>
+    <t>18-01-2020</t>
+  </si>
+  <si>
+    <t>21-01-2020</t>
+  </si>
+  <si>
+    <t>22-01-2020</t>
+  </si>
+  <si>
+    <t>23-01-2020</t>
+  </si>
+  <si>
+    <t>25-01-2020</t>
+  </si>
+  <si>
+    <t>28-01-2020</t>
+  </si>
+  <si>
+    <t>29-01-2020</t>
+  </si>
+  <si>
+    <t>31-01-2020</t>
   </si>
   <si>
     <t/>
@@ -66,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00.00"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="58">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -166,8 +190,144 @@
       <name val="Calibri"/>
       <sz val="12.0"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +391,28 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -484,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment vertical="center" horizontal="center" wrapText="true"/>
@@ -592,66 +774,304 @@
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="44" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="46" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="47" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="18" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment vertical="center" horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="19" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="19" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="164" fontId="21" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="16" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="46" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="47" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="44" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="17" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="13" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="19" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="20" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="51" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="52" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="22" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="54" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="55" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="56" fillId="22" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="57" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment vertical="center" horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="51" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="52" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="23" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="54" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="55" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="56" fillId="23" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="57" fillId="11" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -664,18 +1084,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.05078125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.3359375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="16.4375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.19921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="6.91796875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="6.60546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.82421875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="17.7109375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="24.91015625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="8.57421875" customWidth="true" bestFit="true"/>
@@ -693,7 +1113,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" t="n" s="8">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="2" ht="45.0" customHeight="true">
@@ -732,40 +1152,165 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31"/>
-      <c r="B3" t="s" s="34">
-        <v>14</v>
+      <c r="A3" s="71"/>
+      <c r="B3" t="s" s="102">
+        <v>22</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="31"/>
-      <c r="E3" t="n" s="42">
+      <c r="D3" s="71"/>
+      <c r="E3" t="n" s="110">
+        <v>45.75</v>
+      </c>
+      <c r="F3" t="n" s="111">
         <v>0.0</v>
       </c>
-      <c r="F3" t="n" s="43">
-        <v>0.0</v>
-      </c>
-      <c r="G3" t="n" s="44">
+      <c r="G3" t="n" s="112">
         <v>86.0</v>
       </c>
-      <c r="H3" t="n" s="45">
+      <c r="H3" t="n" s="113">
         <v>20.75</v>
       </c>
-      <c r="I3" t="n" s="46">
+      <c r="I3" t="n" s="114">
         <v>246.0</v>
       </c>
-      <c r="J3" t="n" s="47">
+      <c r="J3" t="n" s="115">
         <v>6.0</v>
       </c>
-      <c r="K3" t="n" s="48">
+      <c r="K3" t="n" s="116">
         <v>252.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" t="s" s="65">
+        <v>13</v>
+      </c>
+      <c r="B4" t="n" s="66">
+        <v>9.0</v>
+      </c>
+      <c r="C4" t="n" s="68">
+        <v>14.0</v>
+      </c>
+      <c r="D4" s="71"/>
+      <c r="E4" t="n" s="75">
+        <v>5.0</v>
+      </c>
+      <c r="F4" s="71"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="67">
+        <v>14</v>
+      </c>
+      <c r="B5" t="n" s="69">
+        <v>14.0</v>
+      </c>
+      <c r="C5" t="n" s="72">
+        <v>19.0</v>
+      </c>
+      <c r="D5" s="71"/>
+      <c r="E5" t="n" s="79">
+        <v>5.0</v>
+      </c>
+      <c r="F5" s="71"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="70">
+        <v>15</v>
+      </c>
+      <c r="B6" t="n" s="73">
+        <v>14.0</v>
+      </c>
+      <c r="C6" t="n" s="76">
+        <v>20.0</v>
+      </c>
+      <c r="D6" s="71"/>
+      <c r="E6" t="n" s="83">
+        <v>6.0</v>
+      </c>
+      <c r="F6" t="n" s="87">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="74">
+        <v>16</v>
+      </c>
+      <c r="B7" t="n" s="77">
+        <v>14.25</v>
+      </c>
+      <c r="C7" t="n" s="80">
+        <v>19.5</v>
+      </c>
+      <c r="D7" s="71"/>
+      <c r="E7" t="n" s="88">
+        <v>5.25</v>
+      </c>
+      <c r="F7" s="71"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="78">
+        <v>17</v>
+      </c>
+      <c r="B8" t="n" s="81">
+        <v>14.0</v>
+      </c>
+      <c r="C8" t="n" s="84">
+        <v>21.5</v>
+      </c>
+      <c r="D8" s="71"/>
+      <c r="E8" t="n" s="92">
+        <v>7.5</v>
+      </c>
+      <c r="F8" t="n" s="95">
+        <v>123.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="82">
+        <v>18</v>
+      </c>
+      <c r="B9" t="n" s="85">
+        <v>9.0</v>
+      </c>
+      <c r="C9" t="n" s="89">
+        <v>19.0</v>
+      </c>
+      <c r="D9" s="71"/>
+      <c r="E9" t="n" s="96">
+        <v>10.0</v>
+      </c>
+      <c r="F9" s="71"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="86">
+        <v>19</v>
+      </c>
+      <c r="B10" t="n" s="90">
+        <v>9.0</v>
+      </c>
+      <c r="C10" t="n" s="93">
+        <v>14.0</v>
+      </c>
+      <c r="D10" s="71"/>
+      <c r="E10" t="n" s="98">
+        <v>5.0</v>
+      </c>
+      <c r="F10" s="71"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="91">
+        <v>20</v>
+      </c>
+      <c r="B11" t="n" s="94">
+        <v>19.0</v>
+      </c>
+      <c r="C11" t="n" s="97">
+        <v>21.0</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" t="n" s="99">
+        <v>2.0</v>
+      </c>
+      <c r="F11" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>